<commit_message>
show items in sidebar
</commit_message>
<xml_diff>
--- a/assets/templates/plantilla-presupuesto-inversiones.xlsx
+++ b/assets/templates/plantilla-presupuesto-inversiones.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keinermolinalemus/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keinermolinalemus/Documents/saber_contable/web-ester/assets/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB920A84-E29C-B848-ADB7-3E8ACF89BC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC875F7-2436-1F45-BA51-AF5CA1527BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="800" windowWidth="36000" windowHeight="21360" xr2:uid="{AD111893-4CF4-3048-BB81-83477B0C9F96}"/>
   </bookViews>
@@ -36,15 +36,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Categoria</t>
+    <t>Plantilla Presupuestos de Inversiones</t>
   </si>
   <si>
-    <t>Monto</t>
+    <t>Descripcion</t>
   </si>
   <si>
-    <t>Plantilla Presupuestos de Inversiones</t>
+    <t>Presupuesto</t>
+  </si>
+  <si>
+    <t>Ejecutado</t>
   </si>
 </sst>
 </file>
@@ -103,7 +106,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -126,12 +129,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -145,13 +185,19 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda [0]" xfId="1" builtinId="7"/>
@@ -490,13 +536,13 @@
   <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" customWidth="1"/>
     <col min="5" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
@@ -526,32 +572,34 @@
       <c r="N1" s="6"/>
     </row>
     <row r="2" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+    </row>
+    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-    </row>
-    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="10" t="s">
-        <v>0</v>
+      <c r="C3" s="8" t="s">
+        <v>3</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="D3" s="9"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -566,7 +614,7 @@
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -582,7 +630,7 @@
       <c r="N4" s="5"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -598,7 +646,7 @@
       <c r="N5" s="5"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -614,7 +662,7 @@
       <c r="N6" s="5"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -630,7 +678,7 @@
       <c r="N7" s="5"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -646,7 +694,7 @@
       <c r="N8" s="5"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -662,7 +710,7 @@
       <c r="N9" s="5"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -678,7 +726,7 @@
       <c r="N10" s="5"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -694,9 +742,9 @@
       <c r="N11" s="5"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
+      <c r="C12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -710,9 +758,9 @@
       <c r="N12" s="6"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
+      <c r="C13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -726,9 +774,9 @@
       <c r="N13" s="6"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
+      <c r="C14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -742,9 +790,9 @@
       <c r="N14" s="6"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
+      <c r="C15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -758,9 +806,9 @@
       <c r="N15" s="6"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
+      <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -774,9 +822,9 @@
       <c r="N16" s="6"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
+      <c r="C17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -792,7 +840,7 @@
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
+      <c r="C18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -1255,7 +1303,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>